<commit_message>
Full metrics; fixed calculating bitrate for adaptive
</commit_message>
<xml_diff>
--- a/results/Huffman_results.xlsx
+++ b/results/Huffman_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\Moje dokumenty\Studia\Semestr 9\KODA\huffman\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\Moje dokumenty\Studia\Semestr 9\KODA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9F770D-5312-474E-840B-3B1DC02F39EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D7073-2D99-464E-B484-8B1171A408BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="3876" windowWidth="22308" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entropy" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>Filename</t>
   </si>
@@ -85,47 +85,54 @@
     <t>uniform.pgm</t>
   </si>
   <si>
-    <t>Entropy</t>
-  </si>
-  <si>
-    <t>Bitrate basic</t>
-  </si>
-  <si>
-    <t>Bitrate adaptive</t>
-  </si>
-  <si>
-    <t>Encode basic [s]</t>
-  </si>
-  <si>
-    <t>Decode basic [s]</t>
-  </si>
-  <si>
-    <t>Encode adaptive [s]</t>
-  </si>
-  <si>
-    <t>Decode adaptive [s]</t>
-  </si>
-  <si>
-    <t>File size [B]</t>
-  </si>
-  <si>
-    <t>Size basic [B]</t>
-  </si>
-  <si>
-    <t>Size adaptive [B]</t>
-  </si>
-  <si>
-    <t>Compression rate basic</t>
-  </si>
-  <si>
-    <t>Compression rate adaptive</t>
+    <t>Nazwa pliku</t>
+  </si>
+  <si>
+    <t>Czas kodowania [s]</t>
+  </si>
+  <si>
+    <t>Algorytm standardowy</t>
+  </si>
+  <si>
+    <t>Algorytm adaptacyjny</t>
+  </si>
+  <si>
+    <t>Czas dekodowania[s]</t>
+  </si>
+  <si>
+    <t>Czas dekodowania [s]</t>
+  </si>
+  <si>
+    <t>Stopień kompresji</t>
+  </si>
+  <si>
+    <t>Standardowy</t>
+  </si>
+  <si>
+    <t>Adaptacyjny</t>
+  </si>
+  <si>
+    <t>Rozmiar pliku po kompresji [B]</t>
+  </si>
+  <si>
+    <t>Rozmiar [B]</t>
+  </si>
+  <si>
+    <t>Entropia</t>
+  </si>
+  <si>
+    <t>Średnia bitowa kodu wyjściowego</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,16 +148,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -173,14 +201,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -498,241 +622,241 @@
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>7.6322382586154749</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>13.324570747812221</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>15.804434555041571</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>7.1916140366645118</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>12.420530951221529</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>15.49522901536905</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>6.1140627573000614</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>9.7103919503402611</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>11.68397170133475</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7.4452551321796356</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12.265045875983891</v>
+      </c>
+      <c r="D5" s="4">
+        <v>15.323594794491861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.2927643468505954</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12.87054997834343</v>
+      </c>
+      <c r="D6" s="4">
+        <v>15.81047485197295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6.7629170705627004</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10.18816755957288</v>
+      </c>
+      <c r="D7" s="6">
+        <v>12.732096536263709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B8" s="5">
         <v>2.0018147001616029</v>
       </c>
-      <c r="C5">
+      <c r="C8" s="5">
         <v>4.0019703011084138</v>
       </c>
-      <c r="D5">
+      <c r="D8" s="5">
         <v>5.9944393172751953</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B9" s="2">
         <v>4.6939553662790319</v>
       </c>
-      <c r="C6">
+      <c r="C9" s="2">
         <v>9.3635693185015416</v>
       </c>
-      <c r="D6">
+      <c r="D9" s="2">
         <v>13.571492945638241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B10" s="2">
         <v>7.6543788986076287</v>
       </c>
-      <c r="C7">
+      <c r="C10" s="2">
         <v>14.93546073085243</v>
       </c>
-      <c r="D7">
+      <c r="D10" s="2">
         <v>16.397433578900259</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B11" s="2">
         <v>5.7677124317963786</v>
       </c>
-      <c r="C8">
+      <c r="C11" s="2">
         <v>11.453615727009369</v>
       </c>
-      <c r="D8">
+      <c r="D11" s="2">
         <v>15.54750072997169</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B12" s="2">
         <v>6.7567224336431568</v>
       </c>
-      <c r="C9">
+      <c r="C12" s="2">
         <v>13.29659603421868</v>
       </c>
-      <c r="D9">
+      <c r="D12" s="2">
         <v>16.25657452317903</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B13" s="2">
         <v>7.2872605823965619</v>
       </c>
-      <c r="C10">
+      <c r="C13" s="2">
         <v>14.259364040226879</v>
       </c>
-      <c r="D10">
+      <c r="D13" s="2">
         <v>16.36463335918662</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>7.4452551321796356</v>
-      </c>
-      <c r="C11">
-        <v>12.265045875983891</v>
-      </c>
-      <c r="D11">
-        <v>15.323594794491861</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>7.2927643468505954</v>
-      </c>
-      <c r="C12">
-        <v>12.87054997834343</v>
-      </c>
-      <c r="D12">
-        <v>15.81047485197295</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="2">
         <v>5.3694020519944479</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="2">
         <v>10.709848561878349</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="2">
         <v>15.174979119776429</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="2">
         <v>6.9546121170383151</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="2">
         <v>13.72540197246806</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="2">
         <v>16.345329890849911</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="2">
         <v>7.649644473403181</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="2">
         <v>14.94053357725134</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="2">
         <v>16.399436388814848</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>6.7629170705627004</v>
-      </c>
-      <c r="C16">
-        <v>10.18816755957288</v>
-      </c>
-      <c r="D16">
-        <v>12.732096536263709</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>7.9993194390339024</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>15.58722646307189</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>16.409752680425701</v>
       </c>
     </row>
@@ -743,928 +867,969 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="11">
         <v>7.6322382586154749</v>
       </c>
-      <c r="C2">
-        <v>8.5276595744680854</v>
-      </c>
-      <c r="D2">
-        <v>8.5319148936170208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" s="11">
+        <v>7.6652096635161824</v>
+      </c>
+      <c r="D3" s="11">
+        <v>7.6776742873271244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="11">
         <v>7.1916140366645118</v>
       </c>
-      <c r="C3">
-        <v>9.1725490196078425</v>
-      </c>
-      <c r="D3">
-        <v>9.1960784313725483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" s="11">
+        <v>7.2189357011541668</v>
+      </c>
+      <c r="D4" s="11">
+        <v>7.232243250871532</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="11">
         <v>6.1140627573000614</v>
       </c>
-      <c r="C4">
-        <v>9.84375</v>
-      </c>
-      <c r="D4">
-        <v>9.84765625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" s="11">
+        <v>6.1313248049065141</v>
+      </c>
+      <c r="D5" s="11">
+        <v>6.1439343662036299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11">
+        <v>7.4452551321796356</v>
+      </c>
+      <c r="C6" s="11">
+        <v>7.4677323386044776</v>
+      </c>
+      <c r="D6" s="11">
+        <v>7.4792434263221734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="11">
+        <v>7.2927643468505954</v>
+      </c>
+      <c r="C7" s="11">
+        <v>7.3190302919346104</v>
+      </c>
+      <c r="D7" s="11">
+        <v>7.3301141954825271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="17">
+        <v>6.7629170705627004</v>
+      </c>
+      <c r="C8" s="17">
+        <v>6.7913472320754291</v>
+      </c>
+      <c r="D8" s="17">
+        <v>6.8003753118063024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B9" s="18">
         <v>2.0018147001616029</v>
       </c>
-      <c r="C5">
-        <v>12.111111111111111</v>
-      </c>
-      <c r="D5">
-        <v>12.148148148148151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C9" s="18">
+        <v>2.001899610541694</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2.002872302686538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B10" s="12">
         <v>4.6939553662790319</v>
       </c>
-      <c r="C6">
-        <v>11.15094339622642</v>
-      </c>
-      <c r="D6">
-        <v>11.16981132075472</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C10" s="12">
+        <v>4.7296793167505173</v>
+      </c>
+      <c r="D10" s="12">
+        <v>4.7348860805846833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B11" s="12">
         <v>7.6543788986076287</v>
       </c>
-      <c r="C7">
-        <v>8.3828125</v>
-      </c>
-      <c r="D7">
-        <v>8.38671875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C11" s="12">
+        <v>7.6827612250580817</v>
+      </c>
+      <c r="D11" s="12">
+        <v>7.6957190102189896</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B12" s="12">
         <v>5.7677124317963786</v>
       </c>
-      <c r="C8">
-        <v>11.74757281553398</v>
-      </c>
-      <c r="D8">
-        <v>11.77669902912621</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C12" s="12">
+        <v>5.8008269790470601</v>
+      </c>
+      <c r="D12" s="12">
+        <v>5.8094057423166854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B13" s="12">
         <v>6.7567224336431568</v>
       </c>
-      <c r="C9">
-        <v>9.87109375</v>
-      </c>
-      <c r="D9">
-        <v>9.875</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C13" s="12">
+        <v>6.7888151846779952</v>
+      </c>
+      <c r="D13" s="12">
+        <v>6.8008269790470672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B14" s="12">
         <v>7.2872605823965619</v>
       </c>
-      <c r="C10">
-        <v>8.890625</v>
-      </c>
-      <c r="D10">
-        <v>8.89453125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>7.4452551321796356</v>
-      </c>
-      <c r="C11">
-        <v>8.5138888888888893</v>
-      </c>
-      <c r="D11">
-        <v>8.5231481481481488</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>7.2927643468505954</v>
-      </c>
-      <c r="C12">
-        <v>9.0714285714285712</v>
-      </c>
-      <c r="D12">
-        <v>9.09375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C14" s="12">
+        <v>7.3138324451954739</v>
+      </c>
+      <c r="D14" s="12">
+        <v>7.3259319725815253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B15" s="12">
         <v>5.3694020519944479</v>
       </c>
-      <c r="C13">
-        <v>9.875</v>
-      </c>
-      <c r="D13">
-        <v>9.8958333333333339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C15" s="12">
+        <v>5.4009284441884509</v>
+      </c>
+      <c r="D15" s="12">
+        <v>5.4051396290037728</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B16" s="12">
         <v>6.9546121170383151</v>
       </c>
-      <c r="C14">
-        <v>10.256198347107439</v>
-      </c>
-      <c r="D14">
-        <v>10.2603305785124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C16" s="12">
+        <v>6.9918751597313076</v>
+      </c>
+      <c r="D16" s="12">
+        <v>7.0031660175694901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B17" s="12">
         <v>7.649644473403181</v>
       </c>
-      <c r="C15">
-        <v>8.5234375</v>
-      </c>
-      <c r="D15">
-        <v>8.52734375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>6.7629170705627004</v>
-      </c>
-      <c r="C16">
-        <v>8.0588235294117645</v>
-      </c>
-      <c r="D16">
-        <v>8.0588235294117645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C17" s="12">
+        <v>7.6711270641099416</v>
+      </c>
+      <c r="D17" s="12">
+        <v>7.6837262882449204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="12">
         <v>7.9993194390339024</v>
       </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>8.00390625</v>
+      <c r="C18" s="12">
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="D18" s="12">
+        <v>8.0138198574147754</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="13">
         <v>0.26261719999999988</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="13">
         <v>2.4387846</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="13">
         <v>3.1098302000000002</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="13">
         <v>2.7910119999999989</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="13">
         <v>0.25921680000000002</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="13">
         <v>2.4171830000000001</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="13">
         <v>2.8891269999999998</v>
       </c>
-      <c r="E3">
+      <c r="E4" s="13">
         <v>0.43443219999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="13">
         <v>0.25621680000000002</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="13">
         <v>2.1310319999999998</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="13">
         <v>2.3931482000000002</v>
       </c>
-      <c r="E4">
+      <c r="E5" s="13">
         <v>2.1185581999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.25962259999999998</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2.4109824</v>
+      </c>
+      <c r="D6" s="13">
+        <v>3.0010241999999998</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2.6275963999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.2632198</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2.4477844000000002</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2.9022242</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2.5863934</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.25741940000000002</v>
+      </c>
+      <c r="C8" s="13">
+        <v>2.2809704000000002</v>
+      </c>
+      <c r="D8" s="13">
+        <v>2.6563987999999998</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2.3114150000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B9" s="14">
         <v>0.24701819999999999</v>
       </c>
-      <c r="C5">
+      <c r="C9" s="14">
         <v>1.0986822000000001</v>
       </c>
-      <c r="D5">
+      <c r="D9" s="14">
         <v>0.92246880000000009</v>
       </c>
-      <c r="E5">
+      <c r="E9" s="14">
         <v>0.89646979999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B10" s="14">
         <v>0.25161899999999998</v>
       </c>
-      <c r="C6">
+      <c r="C10" s="14">
         <v>1.7619313999999999</v>
       </c>
-      <c r="D6">
+      <c r="D10" s="14">
         <v>1.7633684000000001</v>
       </c>
-      <c r="E6">
+      <c r="E10" s="14">
         <v>1.5853208000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B11" s="14">
         <v>0.26741999999999999</v>
       </c>
-      <c r="C7">
+      <c r="C11" s="14">
         <v>2.5115902000000001</v>
       </c>
-      <c r="D7">
+      <c r="D11" s="14">
         <v>3.1762372000000001</v>
       </c>
-      <c r="E7">
+      <c r="E11" s="14">
         <v>2.8392097999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B12" s="14">
         <v>0.25781939999999998</v>
       </c>
-      <c r="C8">
+      <c r="C12" s="14">
         <v>2.0401577999999998</v>
       </c>
-      <c r="D8">
+      <c r="D12" s="14">
         <v>2.1867633999999998</v>
       </c>
-      <c r="E8">
+      <c r="E12" s="14">
         <v>1.9606328</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B13" s="14">
         <v>0.26641759999999998</v>
       </c>
-      <c r="C9">
+      <c r="C13" s="14">
         <v>2.2863707999999998</v>
       </c>
-      <c r="D9">
+      <c r="D13" s="14">
         <v>2.6576010000000001</v>
       </c>
-      <c r="E9">
+      <c r="E13" s="14">
         <v>2.3373746</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B14" s="14">
         <v>0.26281959999999999</v>
       </c>
-      <c r="C10">
+      <c r="C14" s="14">
         <v>2.3841652</v>
       </c>
-      <c r="D10">
+      <c r="D14" s="14">
         <v>3.0972314000000001</v>
       </c>
-      <c r="E10">
+      <c r="E14" s="14">
         <v>2.5957940000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>0.25962259999999998</v>
-      </c>
-      <c r="C11">
-        <v>2.4109824</v>
-      </c>
-      <c r="D11">
-        <v>3.0010241999999998</v>
-      </c>
-      <c r="E11">
-        <v>2.6275963999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>0.2632198</v>
-      </c>
-      <c r="C12">
-        <v>2.4477844000000002</v>
-      </c>
-      <c r="D12">
-        <v>2.9022242</v>
-      </c>
-      <c r="E12">
-        <v>2.5863934</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B15" s="14">
         <v>0.25461919999999999</v>
       </c>
-      <c r="C13">
+      <c r="C15" s="14">
         <v>1.9611487999999999</v>
       </c>
-      <c r="D13">
+      <c r="D15" s="14">
         <v>1.975924</v>
       </c>
-      <c r="E13">
+      <c r="E15" s="14">
         <v>1.7425775999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B16" s="14">
         <v>0.28742159999999989</v>
       </c>
-      <c r="C14">
+      <c r="C16" s="14">
         <v>2.3497754</v>
       </c>
-      <c r="D14">
+      <c r="D16" s="14">
         <v>2.7268059999999998</v>
       </c>
-      <c r="E14">
+      <c r="E16" s="14">
         <v>2.4173827999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B17" s="14">
         <v>0.26301720000000001</v>
       </c>
-      <c r="C15">
+      <c r="C17" s="14">
         <v>2.5103898</v>
       </c>
-      <c r="D15">
+      <c r="D17" s="14">
         <v>3.171637</v>
       </c>
-      <c r="E15">
+      <c r="E17" s="14">
         <v>2.8064076</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>0.25741940000000002</v>
-      </c>
-      <c r="C16">
-        <v>2.2809704000000002</v>
-      </c>
-      <c r="D16">
-        <v>2.6563987999999998</v>
-      </c>
-      <c r="E16">
-        <v>2.3114150000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="14">
         <v>0.26122180000000012</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="14">
         <v>2.4819878000000002</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="14">
         <v>3.5072595999999998</v>
       </c>
-      <c r="E17">
+      <c r="E18" s="14">
         <v>3.1516375999999999</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F18" sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="C1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="19">
         <v>262182</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="19">
         <v>252053</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="19">
         <v>251626</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="20">
         <v>0.96136653164595587</v>
       </c>
-      <c r="F2">
+      <c r="F3" s="20">
         <v>0.95973789199868798</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="9">
         <v>262182</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="9">
         <v>237489</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="9">
         <v>237030</v>
       </c>
-      <c r="E3">
+      <c r="E4" s="11">
         <v>0.90581733299768863</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="11">
         <v>0.90406664073048493</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="9">
         <v>262182</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="9">
         <v>201849</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="9">
         <v>201363</v>
       </c>
-      <c r="E4">
+      <c r="E5" s="11">
         <v>0.76988122754422506</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="11">
         <v>0.76802755337895046</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
+        <v>262182</v>
+      </c>
+      <c r="C6" s="9">
+        <v>245525</v>
+      </c>
+      <c r="D6" s="9">
+        <v>245121</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.93646779717905881</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.93492688285236969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>262182</v>
+      </c>
+      <c r="C7" s="9">
+        <v>240675</v>
+      </c>
+      <c r="D7" s="9">
+        <v>240233</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.91796919697004375</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.91628334515718091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="15">
+        <v>262182</v>
+      </c>
+      <c r="C8" s="15">
+        <v>223170</v>
+      </c>
+      <c r="D8" s="15">
+        <v>222875</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.85120259972080459</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.85007742713077172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B9" s="16">
         <v>262159</v>
       </c>
-      <c r="C5">
+      <c r="C9" s="16">
         <v>65880</v>
       </c>
-      <c r="D5">
+      <c r="D9" s="16">
         <v>65652</v>
       </c>
-      <c r="E5">
+      <c r="E9" s="18">
         <v>0.25129787647954099</v>
       </c>
-      <c r="F5">
+      <c r="F9" s="18">
         <v>0.25042817526768107</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B10" s="10">
         <v>262159</v>
       </c>
-      <c r="C6">
+      <c r="C10" s="10">
         <v>155451</v>
       </c>
-      <c r="D6">
+      <c r="D10" s="10">
         <v>155176</v>
       </c>
-      <c r="E6">
+      <c r="E10" s="12">
         <v>0.59296457493353272</v>
       </c>
-      <c r="F6">
+      <c r="F10" s="12">
         <v>0.59191559320870157</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B11" s="10">
         <v>262159</v>
       </c>
-      <c r="C7">
+      <c r="C11" s="10">
         <v>252670</v>
       </c>
-      <c r="D7">
+      <c r="D11" s="10">
         <v>252196</v>
       </c>
-      <c r="E7">
+      <c r="E11" s="12">
         <v>0.96380440877482754</v>
       </c>
-      <c r="F7">
+      <c r="F11" s="12">
         <v>0.96199634572911863</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B12" s="10">
         <v>262159</v>
       </c>
-      <c r="C8">
+      <c r="C12" s="10">
         <v>190850</v>
       </c>
-      <c r="D8">
+      <c r="D12" s="10">
         <v>190381</v>
       </c>
-      <c r="E8">
+      <c r="E12" s="12">
         <v>0.72799331703279313</v>
       </c>
-      <c r="F8">
+      <c r="F12" s="12">
         <v>0.7262043263820811</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B13" s="10">
         <v>262159</v>
       </c>
-      <c r="C9">
+      <c r="C13" s="10">
         <v>223375</v>
       </c>
-      <c r="D9">
+      <c r="D13" s="10">
         <v>222871</v>
       </c>
-      <c r="E9">
+      <c r="E13" s="12">
         <v>0.8520592464878185</v>
       </c>
-      <c r="F9">
+      <c r="F13" s="12">
         <v>0.850136749072128</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B14" s="10">
         <v>262159</v>
       </c>
-      <c r="C10">
+      <c r="C14" s="10">
         <v>240580</v>
       </c>
-      <c r="D10">
+      <c r="D14" s="10">
         <v>240077</v>
       </c>
-      <c r="E10">
+      <c r="E14" s="12">
         <v>0.91768735767225229</v>
       </c>
-      <c r="F10">
+      <c r="F14" s="12">
         <v>0.91576867473556123</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>262182</v>
-      </c>
-      <c r="C11">
-        <v>245525</v>
-      </c>
-      <c r="D11">
-        <v>245121</v>
-      </c>
-      <c r="E11">
-        <v>0.93646779717905881</v>
-      </c>
-      <c r="F11">
-        <v>0.93492688285236969</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>262182</v>
-      </c>
-      <c r="C12">
-        <v>240675</v>
-      </c>
-      <c r="D12">
-        <v>240233</v>
-      </c>
-      <c r="E12">
-        <v>0.91796919697004375</v>
-      </c>
-      <c r="F12">
-        <v>0.91628334515718091</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B15" s="10">
         <v>262159</v>
       </c>
-      <c r="C13">
+      <c r="C15" s="10">
         <v>177415</v>
       </c>
-      <c r="D13">
+      <c r="D15" s="10">
         <v>177138</v>
       </c>
-      <c r="E13">
+      <c r="E15" s="12">
         <v>0.67674579167604387</v>
       </c>
-      <c r="F13">
+      <c r="F15" s="12">
         <v>0.67568918099321407</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B16" s="10">
         <v>262159</v>
       </c>
-      <c r="C14">
+      <c r="C16" s="10">
         <v>229988</v>
       </c>
-      <c r="D14">
+      <c r="D16" s="10">
         <v>229503</v>
       </c>
-      <c r="E14">
+      <c r="E16" s="12">
         <v>0.87728439611075726</v>
       </c>
-      <c r="F14">
+      <c r="F16" s="12">
         <v>0.87543437379605504</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
+      <c r="B17" s="10">
         <v>262159</v>
       </c>
-      <c r="C15">
+      <c r="C17" s="10">
         <v>252288</v>
       </c>
-      <c r="D15">
+      <c r="D17" s="10">
         <v>251804</v>
       </c>
-      <c r="E15">
+      <c r="E17" s="12">
         <v>0.96234727779706208</v>
       </c>
-      <c r="F15">
+      <c r="F17" s="12">
         <v>0.96050106996135931</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>262182</v>
-      </c>
-      <c r="C16">
-        <v>223170</v>
-      </c>
-      <c r="D16">
-        <v>222875</v>
-      </c>
-      <c r="E16">
-        <v>0.85120259972080459</v>
-      </c>
-      <c r="F16">
-        <v>0.85007742713077172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="10">
         <v>262159</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="10">
         <v>263065</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="10">
         <v>262621</v>
       </c>
-      <c r="E17">
+      <c r="E18" s="12">
         <v>1.0034559179734439</v>
       </c>
-      <c r="F17">
+      <c r="F18" s="12">
         <v>1.001762289297716</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>